<commit_message>
docs: added bolts calculation
</commit_message>
<xml_diff>
--- a/doc/3D_models/Calculation.xlsx
+++ b/doc/3D_models/Calculation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SEEK\SunSensor\druk 3d\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SEEK\SunSensor\sun-sensor-hardware\doc\3D_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="41">
   <si>
     <t>sensor length</t>
   </si>
@@ -113,10 +113,40 @@
     <t>To</t>
   </si>
   <si>
-    <t>VERSION 4</t>
-  </si>
-  <si>
     <t>VERSION 2-3</t>
+  </si>
+  <si>
+    <t>VERSION 4-6</t>
+  </si>
+  <si>
+    <t>Bolt size</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>Nut size</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Borders</t>
+  </si>
+  <si>
+    <t>Length S</t>
+  </si>
+  <si>
+    <t>Length L</t>
   </si>
 </sst>
 </file>
@@ -177,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -186,6 +216,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -473,7 +507,7 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,28 +520,28 @@
     <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="4.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
+      <c r="A1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -752,21 +786,21 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
+      <c r="A14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -955,6 +989,21 @@
       <c r="D21" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="I21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -970,6 +1019,21 @@
       <c r="D22" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="I22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="K22" s="3">
+        <v>10</v>
+      </c>
+      <c r="L22" s="3">
+        <v>20</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
@@ -985,6 +1049,21 @@
       <c r="D23" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="I23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
@@ -1007,6 +1086,21 @@
         <v>5.3999999999999995</v>
       </c>
       <c r="G24" t="s">
+        <v>6</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J24" s="3">
+        <v>6</v>
+      </c>
+      <c r="K24" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="L24" s="3">
+        <v>5.4</v>
+      </c>
+      <c r="M24" s="3" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
docs: added frame stick V2 and slit sensor face V7
</commit_message>
<xml_diff>
--- a/doc/3D_models/Calculation.xlsx
+++ b/doc/3D_models/Calculation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="42">
   <si>
     <t>sensor length</t>
   </si>
@@ -116,9 +116,6 @@
     <t>VERSION 2-3</t>
   </si>
   <si>
-    <t>VERSION 4-6</t>
-  </si>
-  <si>
     <t>Bolt size</t>
   </si>
   <si>
@@ -147,6 +144,12 @@
   </si>
   <si>
     <t>Length L</t>
+  </si>
+  <si>
+    <t>VERSION 4-…</t>
+  </si>
+  <si>
+    <t>Length</t>
   </si>
 </sst>
 </file>
@@ -207,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -224,6 +227,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -504,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T28" sqref="T28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,7 +527,8 @@
     <col min="10" max="10" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -787,7 +792,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -863,7 +868,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>1</v>
       </c>
@@ -895,7 +900,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>12</v>
       </c>
@@ -927,7 +932,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>13</v>
       </c>
@@ -960,7 +965,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>16</v>
       </c>
@@ -975,7 +980,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>15</v>
       </c>
@@ -990,22 +995,22 @@
         <v>6</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L21" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>18</v>
       </c>
@@ -1020,10 +1025,10 @@
         <v>6</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K22" s="3">
         <v>10</v>
@@ -1035,7 +1040,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -1050,22 +1055,25 @@
         <v>6</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="M23" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M23" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="N23" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>22</v>
       </c>
@@ -1089,7 +1097,7 @@
         <v>6</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J24" s="3">
         <v>6</v>
@@ -1100,7 +1108,10 @@
       <c r="L24" s="3">
         <v>5.4</v>
       </c>
-      <c r="M24" s="3" t="s">
+      <c r="M24" s="8">
+        <v>6</v>
+      </c>
+      <c r="N24" s="3" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
docs: added internal platform v3, update excel calculator  and readme
</commit_message>
<xml_diff>
--- a/doc/3D_models/Calculation.xlsx
+++ b/doc/3D_models/Calculation.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13185" windowHeight="10725"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13185" windowHeight="10725" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="Face" sheetId="1" r:id="rId1"/>
+    <sheet name="Platform" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="56">
   <si>
     <t>sensor length</t>
   </si>
@@ -150,13 +151,55 @@
   </si>
   <si>
     <t>Length</t>
+  </si>
+  <si>
+    <t>Dimension</t>
+  </si>
+  <si>
+    <t>Circuit board</t>
+  </si>
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>Top</t>
+  </si>
+  <si>
+    <t>Bottom</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Front</t>
+  </si>
+  <si>
+    <t>Projection</t>
+  </si>
+  <si>
+    <t>Platform slit</t>
+  </si>
+  <si>
+    <t>VERSION 1-…</t>
+  </si>
+  <si>
+    <t>Spacing bettwen Circuit board and Platform slit</t>
+  </si>
+  <si>
+    <t>Circuit board support stand</t>
+  </si>
+  <si>
+    <t>Empty slit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,6 +211,15 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -210,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -224,10 +276,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -510,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T28" sqref="T28"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,22 +586,22 @@
     <col min="14" max="14" width="4.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -790,22 +845,22 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+    <row r="14" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+      <c r="A14" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -1108,7 +1163,7 @@
       <c r="L24" s="3">
         <v>5.4</v>
       </c>
-      <c r="M24" s="8">
+      <c r="M24" s="7">
         <v>6</v>
       </c>
       <c r="N24" s="3" t="s">
@@ -1123,4 +1178,354 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AF13" sqref="AF13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="E3" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="J3" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="N3" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="S3" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="3">
+        <v>51</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="3">
+        <f>B5+G5+G6</f>
+        <v>53</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="P5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="T5" s="3">
+        <f>B5-P5-P6</f>
+        <v>51</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="3">
+        <v>51</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" s="3">
+        <f>B6+G7+G8</f>
+        <v>53</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="P6" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="T6" s="3">
+        <f>B6-P7-P8</f>
+        <v>48.599999999999994</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="3">
+        <f>B7+G9+G10</f>
+        <v>1.2</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="P7" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="P8" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="S3:U3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added internal platform v3, update excel calculator and readme
</commit_message>
<xml_diff>
--- a/doc/3D_models/Calculation.xlsx
+++ b/doc/3D_models/Calculation.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="60">
   <si>
     <t>sensor length</t>
   </si>
@@ -193,6 +193,19 @@
   </si>
   <si>
     <t>Empty slit</t>
+  </si>
+  <si>
+    <t>VERSION 3-…</t>
+  </si>
+  <si>
+    <t>Platform board thickness</t>
+  </si>
+  <si>
+    <t>Platform size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grid pattern   
+</t>
   </si>
 </sst>
 </file>
@@ -235,7 +248,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -258,11 +271,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -277,11 +336,37 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -587,21 +672,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -846,21 +931,21 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -1182,10 +1267,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U10"/>
+  <dimension ref="A1:Y22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF13" sqref="AF13"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1198,54 +1283,65 @@
     <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:25" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="E3" s="8" t="s">
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="E3" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="J3" s="8" t="s">
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="J3" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="N3" s="8" t="s">
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="N3" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="S3" s="8" t="s">
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="S3" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>42</v>
       </c>
@@ -1298,7 +1394,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>41</v>
       </c>
@@ -1353,7 +1449,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>34</v>
       </c>
@@ -1408,7 +1504,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>35</v>
       </c>
@@ -1462,7 +1558,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E8" s="3" t="s">
         <v>45</v>
       </c>
@@ -1488,7 +1584,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E9" s="3" t="s">
         <v>49</v>
       </c>
@@ -1502,7 +1598,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E10" s="3" t="s">
         <v>49</v>
       </c>
@@ -1516,14 +1612,393 @@
         <v>6</v>
       </c>
     </row>
+    <row r="13" spans="1:25" ht="21" x14ac:dyDescent="0.35">
+      <c r="A13" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="S14" s="13"/>
+      <c r="T14" s="13"/>
+      <c r="U14" s="13"/>
+      <c r="V14" s="13"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="E15" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="J15" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="N15" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="12"/>
+      <c r="W15" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="X15" s="11"/>
+      <c r="Y15" s="12"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P16" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q16" s="20"/>
+      <c r="R16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="T16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="W16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="X16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y16" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="3">
+        <v>54</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K17" s="3">
+        <f>B17+G17+G18</f>
+        <v>54</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O17" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="P17" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q17" s="21"/>
+      <c r="R17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="S17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="T17" s="3">
+        <v>1</v>
+      </c>
+      <c r="U17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="W17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="X17" s="3">
+        <f>K17+T17+T18</f>
+        <v>56</v>
+      </c>
+      <c r="Y17" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="3">
+        <v>51</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K18" s="3">
+        <f>B18+G19+G20</f>
+        <v>51</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N18" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="22"/>
+      <c r="R18" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="S18" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="T18" s="3">
+        <v>1</v>
+      </c>
+      <c r="U18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="W18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="X18" s="3">
+        <f>K18+T19+T20</f>
+        <v>56</v>
+      </c>
+      <c r="Y18" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K19" s="3">
+        <f>B19+G21+G22</f>
+        <v>1.2</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N19" s="23"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="18"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="S19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="T19" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="U19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="W19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="X19" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="Y19" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="E20" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="S20" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="T20" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="U20" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="E21" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="E22" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="14">
+    <mergeCell ref="W15:Y15"/>
+    <mergeCell ref="R15:U15"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="N15:P15"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="A1:U1"/>
+    <mergeCell ref="A13:U13"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="J15:L15"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="E3:H3"/>
     <mergeCell ref="J3:L3"/>
-    <mergeCell ref="A1:L1"/>
     <mergeCell ref="N3:Q3"/>
-    <mergeCell ref="S3:U3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
docs: added internal platform v4, update excel and readme
</commit_message>
<xml_diff>
--- a/doc/3D_models/Calculation.xlsx
+++ b/doc/3D_models/Calculation.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="61">
   <si>
     <t>sensor length</t>
   </si>
@@ -205,6 +205,10 @@
   </si>
   <si>
     <t xml:space="preserve">grid pattern   
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grid pattern mechd with pads
 </t>
   </si>
 </sst>
@@ -212,7 +216,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,6 +238,13 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -321,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -336,10 +347,18 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -351,22 +370,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -672,21 +689,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -931,21 +948,21 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -1267,10 +1284,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y22"/>
+  <dimension ref="A1:Y34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="Z33" sqref="Z33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1288,58 +1305,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="E3" s="9" t="s">
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="E3" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="J3" s="9" t="s">
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="J3" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="N3" s="9" t="s">
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="N3" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="S3" s="9" t="s">
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="S3" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="T3" s="9"/>
-      <c r="U3" s="9"/>
+      <c r="T3" s="23"/>
+      <c r="U3" s="23"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1613,70 +1630,70 @@
       </c>
     </row>
     <row r="13" spans="1:25" ht="21" x14ac:dyDescent="0.35">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
-      <c r="U13" s="8"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="17"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="17"/>
+      <c r="S13" s="17"/>
+      <c r="T13" s="17"/>
+      <c r="U13" s="17"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="S14" s="13"/>
-      <c r="T14" s="13"/>
-      <c r="U14" s="13"/>
-      <c r="V14" s="13"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="E15" s="9" t="s">
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="E15" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="J15" s="9" t="s">
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="J15" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="N15" s="10" t="s">
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="N15" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="19"/>
-      <c r="R15" s="10" t="s">
+      <c r="O15" s="19"/>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="S15" s="11"/>
-      <c r="T15" s="11"/>
-      <c r="U15" s="12"/>
-      <c r="W15" s="10" t="s">
+      <c r="S15" s="19"/>
+      <c r="T15" s="19"/>
+      <c r="U15" s="20"/>
+      <c r="W15" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="X15" s="11"/>
-      <c r="Y15" s="12"/>
+      <c r="X15" s="19"/>
+      <c r="Y15" s="20"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -1715,10 +1732,10 @@
       <c r="O16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P16" s="16" t="s">
+      <c r="P16" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="Q16" s="20"/>
+      <c r="Q16" s="13"/>
       <c r="R16" s="2" t="s">
         <v>50</v>
       </c>
@@ -1779,10 +1796,10 @@
       <c r="O17" s="3">
         <v>0.8</v>
       </c>
-      <c r="P17" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q17" s="21"/>
+      <c r="P17" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q17" s="14"/>
       <c r="R17" s="3" t="s">
         <v>45</v>
       </c>
@@ -1838,12 +1855,12 @@
       <c r="L18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="N18" s="14" t="s">
+      <c r="N18" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="O18" s="15"/>
-      <c r="P18" s="15"/>
-      <c r="Q18" s="22"/>
+      <c r="O18" s="22"/>
+      <c r="P18" s="22"/>
+      <c r="Q18" s="15"/>
       <c r="R18" s="3" t="s">
         <v>45</v>
       </c>
@@ -1899,10 +1916,10 @@
       <c r="L19" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="N19" s="23"/>
-      <c r="O19" s="18"/>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="18"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
       <c r="R19" s="3" t="s">
         <v>45</v>
       </c>
@@ -1938,10 +1955,10 @@
       <c r="H20" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="13"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
       <c r="R20" s="3" t="s">
         <v>45</v>
       </c>
@@ -1983,13 +2000,381 @@
         <v>6</v>
       </c>
     </row>
+    <row r="25" spans="1:25" ht="21" x14ac:dyDescent="0.35">
+      <c r="A25" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="17"/>
+      <c r="M25" s="17"/>
+      <c r="N25" s="17"/>
+      <c r="O25" s="17"/>
+      <c r="P25" s="17"/>
+      <c r="Q25" s="17"/>
+      <c r="R25" s="17"/>
+      <c r="S25" s="17"/>
+      <c r="T25" s="17"/>
+      <c r="U25" s="17"/>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A27" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="E27" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="J27" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="K27" s="23"/>
+      <c r="L27" s="23"/>
+      <c r="N27" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="O27" s="19"/>
+      <c r="P27" s="19"/>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="S27" s="19"/>
+      <c r="T27" s="19"/>
+      <c r="U27" s="20"/>
+      <c r="W27" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="X27" s="19"/>
+      <c r="Y27" s="20"/>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P28" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q28" s="13"/>
+      <c r="R28" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S28" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="T28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="W28" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="X28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y28" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="3">
+        <v>54</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G29" s="3">
+        <v>0</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K29" s="3">
+        <f>B29+G29+G30</f>
+        <v>54</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N29" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O29" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="P29" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q29" s="14"/>
+      <c r="R29" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="S29" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="T29" s="3">
+        <v>1</v>
+      </c>
+      <c r="U29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="W29" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="X29" s="3">
+        <f>K29+T29+T30</f>
+        <v>56</v>
+      </c>
+      <c r="Y29" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" s="3">
+        <v>50</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G30" s="3">
+        <v>0</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K30" s="3">
+        <f>B30+G31+G32</f>
+        <v>50</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N30" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="O30" s="25"/>
+      <c r="P30" s="25"/>
+      <c r="Q30" s="15"/>
+      <c r="R30" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="S30" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="T30" s="3">
+        <v>1</v>
+      </c>
+      <c r="U30" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="W30" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="X30" s="3">
+        <f>K30+T31+T32</f>
+        <v>56</v>
+      </c>
+      <c r="Y30" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G31" s="3">
+        <v>0</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K31" s="3">
+        <f>B31+G33+G34</f>
+        <v>1.2</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N31" s="16"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="11"/>
+      <c r="R31" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="S31" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="T31" s="3">
+        <v>3</v>
+      </c>
+      <c r="U31" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="W31" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="X31" s="3">
+        <v>2</v>
+      </c>
+      <c r="Y31" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="E32" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G32" s="3">
+        <v>0</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N32" s="8"/>
+      <c r="O32" s="8"/>
+      <c r="P32" s="8"/>
+      <c r="Q32" s="8"/>
+      <c r="R32" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="S32" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="T32" s="3">
+        <v>3</v>
+      </c>
+      <c r="U32" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E33" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G33" s="3">
+        <v>0</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E34" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G34" s="3">
+        <v>0</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="W15:Y15"/>
-    <mergeCell ref="R15:U15"/>
-    <mergeCell ref="N18:P18"/>
-    <mergeCell ref="N15:P15"/>
-    <mergeCell ref="S3:U3"/>
+  <mergeCells count="22">
+    <mergeCell ref="W27:Y27"/>
+    <mergeCell ref="N30:P30"/>
+    <mergeCell ref="A25:U25"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="E27:H27"/>
+    <mergeCell ref="J27:L27"/>
+    <mergeCell ref="N27:P27"/>
+    <mergeCell ref="R27:U27"/>
     <mergeCell ref="A1:U1"/>
     <mergeCell ref="A13:U13"/>
     <mergeCell ref="A15:C15"/>
@@ -1999,6 +2384,11 @@
     <mergeCell ref="E3:H3"/>
     <mergeCell ref="J3:L3"/>
     <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="W15:Y15"/>
+    <mergeCell ref="R15:U15"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="N15:P15"/>
+    <mergeCell ref="S3:U3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
feat: add slit sensor face v8 calculations
</commit_message>
<xml_diff>
--- a/doc/3D_models/Calculation.xlsx
+++ b/doc/3D_models/Calculation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13185" windowHeight="10725" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13185" windowHeight="10725"/>
   </bookViews>
   <sheets>
     <sheet name="Face" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="78">
   <si>
     <t>sensor length</t>
   </si>
@@ -210,6 +210,57 @@
   <si>
     <t xml:space="preserve">grid pattern mechd with pads
 </t>
+  </si>
+  <si>
+    <t>VERSION 8-…</t>
+  </si>
+  <si>
+    <t>Board raster</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>Sensor spacing to board</t>
+  </si>
+  <si>
+    <t>sensor length (max)</t>
+  </si>
+  <si>
+    <t>sensor width (max)</t>
+  </si>
+  <si>
+    <t>Sensor height (avg)</t>
+  </si>
+  <si>
+    <t>Sensor height to board</t>
+  </si>
+  <si>
+    <t>Face height</t>
+  </si>
+  <si>
+    <t>Separator slot</t>
+  </si>
+  <si>
+    <t>Separator height</t>
+  </si>
+  <si>
+    <t>From separator slot to array</t>
+  </si>
+  <si>
+    <t>From separator slot to board</t>
+  </si>
+  <si>
+    <t>From face bottom to array</t>
+  </si>
+  <si>
+    <t>From face bottom to board</t>
+  </si>
+  <si>
+    <t>From face top to array</t>
+  </si>
+  <si>
+    <t>From face top to board</t>
   </si>
 </sst>
 </file>
@@ -332,7 +383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -358,6 +409,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -370,20 +429,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -400,6 +459,66 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>277585</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>163285</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>506185</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>125185</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Obraz 1" descr="https://lh7-rt.googleusercontent.com/docsz/AD_4nXeKu-IH9_Nq2-O2HdGNxbT3_GdBck_ah4-QxpathXNl3Ulcg0JIx0JRMbdK4V0Ue0IHN7uHGO4qgw-x_vpy2QhlXqJiGxW2M1ltXuNpfxcKIsA3ggSjSjGAxpyBrr6T8n_P_Gp_?key=38QlTr_chWmi926Jp3nq1fbq"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9516835" y="1006928"/>
+          <a:ext cx="4623707" cy="3663043"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -665,17 +784,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:U37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V24" sqref="V24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
@@ -686,24 +805,31 @@
     <col min="12" max="12" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5" customWidth="1"/>
+    <col min="16" max="16" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.5703125" customWidth="1"/>
+    <col min="19" max="19" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.42578125" customWidth="1"/>
+    <col min="21" max="21" width="4.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -948,21 +1074,21 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -1025,7 +1151,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>1</v>
       </c>
@@ -1057,7 +1183,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>12</v>
       </c>
@@ -1089,7 +1215,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>13</v>
       </c>
@@ -1122,7 +1248,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>16</v>
       </c>
@@ -1137,7 +1263,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>15</v>
       </c>
@@ -1167,7 +1293,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>18</v>
       </c>
@@ -1197,7 +1323,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -1230,7 +1356,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>22</v>
       </c>
@@ -1272,13 +1398,489 @@
         <v>6</v>
       </c>
     </row>
+    <row r="27" spans="1:21" ht="21" x14ac:dyDescent="0.35">
+      <c r="A27" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
+      <c r="L27" s="21"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="21"/>
+      <c r="O27" s="21"/>
+      <c r="P27" s="21"/>
+      <c r="Q27" s="21"/>
+      <c r="R27" s="21"/>
+      <c r="S27" s="21"/>
+      <c r="T27" s="21"/>
+      <c r="U27" s="21"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I28" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J28" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="K28" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="L28" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="M28" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="P28" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q28" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="T28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U28" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I29" s="3">
+        <v>1</v>
+      </c>
+      <c r="J29" s="3">
+        <f>K29-$C$29/2</f>
+        <v>-9.870000000000001</v>
+      </c>
+      <c r="K29" s="3">
+        <f>$P$29*-3</f>
+        <v>-7.62</v>
+      </c>
+      <c r="L29" s="3">
+        <f>K29+$C$29/2</f>
+        <v>-5.37</v>
+      </c>
+      <c r="M29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P29" s="3">
+        <v>2.54</v>
+      </c>
+      <c r="Q29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S29" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="T29" s="3">
+        <v>2</v>
+      </c>
+      <c r="U29" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="3">
+        <v>5.2</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I30" s="3">
+        <v>2</v>
+      </c>
+      <c r="J30" s="3">
+        <f t="shared" ref="J30:J32" si="0">K30-$C$29/2</f>
+        <v>-4.79</v>
+      </c>
+      <c r="K30" s="3">
+        <f>$P$29*-1</f>
+        <v>-2.54</v>
+      </c>
+      <c r="L30" s="3">
+        <f t="shared" ref="L30:L32" si="1">K30+$C$29/2</f>
+        <v>-0.29000000000000004</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S30" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="T30" s="19">
+        <v>0.4</v>
+      </c>
+      <c r="U30" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="3">
+        <v>4</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I31" s="3">
+        <v>3</v>
+      </c>
+      <c r="J31" s="3">
+        <f t="shared" si="0"/>
+        <v>0.29000000000000004</v>
+      </c>
+      <c r="K31" s="3">
+        <f>$P$29*1</f>
+        <v>2.54</v>
+      </c>
+      <c r="L31" s="3">
+        <f t="shared" si="1"/>
+        <v>4.79</v>
+      </c>
+      <c r="M31" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S31" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="T31" s="3">
+        <f>C34+P37-T29+T30</f>
+        <v>10.570000000000002</v>
+      </c>
+      <c r="U31" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="3">
+        <f>ABS(J29-L32)</f>
+        <v>19.740000000000002</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I32" s="3">
+        <v>4</v>
+      </c>
+      <c r="J32" s="3">
+        <f t="shared" si="0"/>
+        <v>5.37</v>
+      </c>
+      <c r="K32" s="3">
+        <f>$P$29*3</f>
+        <v>7.62</v>
+      </c>
+      <c r="L32" s="3">
+        <f t="shared" si="1"/>
+        <v>9.870000000000001</v>
+      </c>
+      <c r="M32" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O32" s="18"/>
+      <c r="P32" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q32" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="S32" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="T32" s="19">
+        <f>C34-T29</f>
+        <v>7.870000000000001</v>
+      </c>
+      <c r="U32" s="20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="3">
+        <f>C32/2</f>
+        <v>9.870000000000001</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P33" s="3">
+        <f>1.9 + ABS(1.9 - 2.3) / 2</f>
+        <v>2.0999999999999996</v>
+      </c>
+      <c r="Q33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S33" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="T33" s="3">
+        <f>C34-T29+P37</f>
+        <v>10.170000000000002</v>
+      </c>
+      <c r="U33" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="3">
+        <f>C32/2</f>
+        <v>9.870000000000001</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P34" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q34" s="5"/>
+      <c r="S34" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="T34" s="19">
+        <f>C34-(T29+T30)</f>
+        <v>7.4700000000000006</v>
+      </c>
+      <c r="U34" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" s="3">
+        <f>2*C34</f>
+        <v>19.740000000000002</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J35" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K35" s="3">
+        <v>10</v>
+      </c>
+      <c r="L35" s="3">
+        <v>20</v>
+      </c>
+      <c r="M35" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P35" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="Q35" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S35" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="T35" s="3">
+        <f>C34-(T29+T30)+P37</f>
+        <v>9.77</v>
+      </c>
+      <c r="U35" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="3">
+        <f>C29*0.8</f>
+        <v>3.6</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L36" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M36" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="N36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P36" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q36" s="5"/>
+      <c r="S36" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="T36" s="19">
+        <f>C34</f>
+        <v>9.870000000000001</v>
+      </c>
+      <c r="U36" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F37">
+        <f>C36/TAN(45)</f>
+        <v>2.2225306456207981</v>
+      </c>
+      <c r="G37" t="s">
+        <v>6</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J37" s="3">
+        <v>6</v>
+      </c>
+      <c r="K37" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="L37" s="3">
+        <v>5.4</v>
+      </c>
+      <c r="M37" s="7">
+        <v>6</v>
+      </c>
+      <c r="N37" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P37" s="3">
+        <f>P33+P35</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Q37" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S37" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="T37" s="3">
+        <f>C34+P37</f>
+        <v>12.170000000000002</v>
+      </c>
+      <c r="U37" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="A14:M14"/>
+    <mergeCell ref="A27:U27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1286,8 +1888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z33" sqref="Z33"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1305,58 +1907,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="17"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="21"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="E3" s="23" t="s">
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="E3" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="J3" s="23" t="s">
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="J3" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="N3" s="23" t="s">
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="N3" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="23"/>
-      <c r="S3" s="23" t="s">
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="27"/>
+      <c r="S3" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="T3" s="23"/>
-      <c r="U3" s="23"/>
+      <c r="T3" s="27"/>
+      <c r="U3" s="27"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1630,29 +2232,29 @@
       </c>
     </row>
     <row r="13" spans="1:25" ht="21" x14ac:dyDescent="0.35">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="17"/>
-      <c r="P13" s="17"/>
-      <c r="Q13" s="17"/>
-      <c r="R13" s="17"/>
-      <c r="S13" s="17"/>
-      <c r="T13" s="17"/>
-      <c r="U13" s="17"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="21"/>
+      <c r="Q13" s="21"/>
+      <c r="R13" s="21"/>
+      <c r="S13" s="21"/>
+      <c r="T13" s="21"/>
+      <c r="U13" s="21"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="S14" s="8"/>
@@ -1661,39 +2263,39 @@
       <c r="V14" s="8"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="E15" s="23" t="s">
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="E15" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="J15" s="23" t="s">
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="J15" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="K15" s="23"/>
-      <c r="L15" s="23"/>
-      <c r="N15" s="18" t="s">
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
+      <c r="N15" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="O15" s="19"/>
-      <c r="P15" s="19"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="23"/>
       <c r="Q15" s="12"/>
-      <c r="R15" s="18" t="s">
+      <c r="R15" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="S15" s="19"/>
-      <c r="T15" s="19"/>
-      <c r="U15" s="20"/>
-      <c r="W15" s="18" t="s">
+      <c r="S15" s="23"/>
+      <c r="T15" s="23"/>
+      <c r="U15" s="24"/>
+      <c r="W15" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="X15" s="19"/>
-      <c r="Y15" s="20"/>
+      <c r="X15" s="23"/>
+      <c r="Y15" s="24"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -1855,11 +2457,11 @@
       <c r="L18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="N18" s="21" t="s">
+      <c r="N18" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="O18" s="22"/>
-      <c r="P18" s="22"/>
+      <c r="O18" s="29"/>
+      <c r="P18" s="29"/>
       <c r="Q18" s="15"/>
       <c r="R18" s="3" t="s">
         <v>45</v>
@@ -2001,64 +2603,64 @@
       </c>
     </row>
     <row r="25" spans="1:25" ht="21" x14ac:dyDescent="0.35">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="17"/>
-      <c r="L25" s="17"/>
-      <c r="M25" s="17"/>
-      <c r="N25" s="17"/>
-      <c r="O25" s="17"/>
-      <c r="P25" s="17"/>
-      <c r="Q25" s="17"/>
-      <c r="R25" s="17"/>
-      <c r="S25" s="17"/>
-      <c r="T25" s="17"/>
-      <c r="U25" s="17"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="21"/>
+      <c r="Q25" s="21"/>
+      <c r="R25" s="21"/>
+      <c r="S25" s="21"/>
+      <c r="T25" s="21"/>
+      <c r="U25" s="21"/>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="E27" s="23" t="s">
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="E27" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
-      <c r="J27" s="23" t="s">
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="J27" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="K27" s="23"/>
-      <c r="L27" s="23"/>
-      <c r="N27" s="18" t="s">
+      <c r="K27" s="27"/>
+      <c r="L27" s="27"/>
+      <c r="N27" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="O27" s="19"/>
-      <c r="P27" s="19"/>
+      <c r="O27" s="23"/>
+      <c r="P27" s="23"/>
       <c r="Q27" s="12"/>
-      <c r="R27" s="18" t="s">
+      <c r="R27" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="S27" s="19"/>
-      <c r="T27" s="19"/>
-      <c r="U27" s="20"/>
-      <c r="W27" s="18" t="s">
+      <c r="S27" s="23"/>
+      <c r="T27" s="23"/>
+      <c r="U27" s="24"/>
+      <c r="W27" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="X27" s="19"/>
-      <c r="Y27" s="20"/>
+      <c r="X27" s="23"/>
+      <c r="Y27" s="24"/>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
@@ -2220,11 +2822,11 @@
       <c r="L30" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="N30" s="24" t="s">
+      <c r="N30" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="O30" s="25"/>
-      <c r="P30" s="25"/>
+      <c r="O30" s="26"/>
+      <c r="P30" s="26"/>
       <c r="Q30" s="15"/>
       <c r="R30" s="3" t="s">
         <v>45</v>
@@ -2367,14 +2969,11 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="W27:Y27"/>
-    <mergeCell ref="N30:P30"/>
-    <mergeCell ref="A25:U25"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="E27:H27"/>
-    <mergeCell ref="J27:L27"/>
-    <mergeCell ref="N27:P27"/>
-    <mergeCell ref="R27:U27"/>
+    <mergeCell ref="W15:Y15"/>
+    <mergeCell ref="R15:U15"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="N15:P15"/>
+    <mergeCell ref="S3:U3"/>
     <mergeCell ref="A1:U1"/>
     <mergeCell ref="A13:U13"/>
     <mergeCell ref="A15:C15"/>
@@ -2384,11 +2983,14 @@
     <mergeCell ref="E3:H3"/>
     <mergeCell ref="J3:L3"/>
     <mergeCell ref="N3:Q3"/>
-    <mergeCell ref="W15:Y15"/>
-    <mergeCell ref="R15:U15"/>
-    <mergeCell ref="N18:P18"/>
-    <mergeCell ref="N15:P15"/>
-    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="W27:Y27"/>
+    <mergeCell ref="N30:P30"/>
+    <mergeCell ref="A25:U25"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="E27:H27"/>
+    <mergeCell ref="J27:L27"/>
+    <mergeCell ref="N27:P27"/>
+    <mergeCell ref="R27:U27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
feat: update calculation sheet, create SunSensor v2.0 parts: `Slit Sensor Face v8` and `Frame Stick v4`
</commit_message>
<xml_diff>
--- a/doc/3D_models/Calculation.xlsx
+++ b/doc/3D_models/Calculation.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="79">
   <si>
     <t>sensor length</t>
   </si>
@@ -261,6 +261,9 @@
   </si>
   <si>
     <t>From face top to board</t>
+  </si>
+  <si>
+    <t>M1.6</t>
   </si>
 </sst>
 </file>
@@ -429,20 +432,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -786,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V24" sqref="V24"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1697,10 +1700,10 @@
         <v>33</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="M34" s="2" t="s">
         <v>5</v>
@@ -1738,13 +1741,13 @@
         <v>36</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="K35" s="3">
-        <v>10</v>
-      </c>
-      <c r="L35" s="3">
-        <v>20</v>
+        <v>16</v>
+      </c>
+      <c r="L35">
+        <v>1.3</v>
       </c>
       <c r="M35" s="3" t="s">
         <v>6</v>
@@ -1843,13 +1846,13 @@
         <v>6</v>
       </c>
       <c r="K37" s="3">
-        <v>2.4</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="L37" s="3">
-        <v>5.4</v>
+        <v>3</v>
       </c>
       <c r="M37" s="7">
-        <v>6</v>
+        <v>3.4</v>
       </c>
       <c r="N37" s="3" t="s">
         <v>6</v>
@@ -2457,11 +2460,11 @@
       <c r="L18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="N18" s="28" t="s">
+      <c r="N18" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="O18" s="29"/>
-      <c r="P18" s="29"/>
+      <c r="O18" s="26"/>
+      <c r="P18" s="26"/>
       <c r="Q18" s="15"/>
       <c r="R18" s="3" t="s">
         <v>45</v>
@@ -2822,11 +2825,11 @@
       <c r="L30" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="N30" s="25" t="s">
+      <c r="N30" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="O30" s="26"/>
-      <c r="P30" s="26"/>
+      <c r="O30" s="29"/>
+      <c r="P30" s="29"/>
       <c r="Q30" s="15"/>
       <c r="R30" s="3" t="s">
         <v>45</v>
@@ -2969,11 +2972,14 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="W15:Y15"/>
-    <mergeCell ref="R15:U15"/>
-    <mergeCell ref="N18:P18"/>
-    <mergeCell ref="N15:P15"/>
-    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="W27:Y27"/>
+    <mergeCell ref="N30:P30"/>
+    <mergeCell ref="A25:U25"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="E27:H27"/>
+    <mergeCell ref="J27:L27"/>
+    <mergeCell ref="N27:P27"/>
+    <mergeCell ref="R27:U27"/>
     <mergeCell ref="A1:U1"/>
     <mergeCell ref="A13:U13"/>
     <mergeCell ref="A15:C15"/>
@@ -2983,14 +2989,11 @@
     <mergeCell ref="E3:H3"/>
     <mergeCell ref="J3:L3"/>
     <mergeCell ref="N3:Q3"/>
-    <mergeCell ref="W27:Y27"/>
-    <mergeCell ref="N30:P30"/>
-    <mergeCell ref="A25:U25"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="E27:H27"/>
-    <mergeCell ref="J27:L27"/>
-    <mergeCell ref="N27:P27"/>
-    <mergeCell ref="R27:U27"/>
+    <mergeCell ref="W15:Y15"/>
+    <mergeCell ref="R15:U15"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="N15:P15"/>
+    <mergeCell ref="S3:U3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>